<commit_message>
Add new survey error
</commit_message>
<xml_diff>
--- a/EmployeeEvaluation/bledy.xlsx
+++ b/EmployeeEvaluation/bledy.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kasia\source\repos\EmployeeEvaluation\EmployeeEvaluation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Grzesiek\source\repos\EmployeeEvaluation\EmployeeEvaluation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{A8B81856-FF95-4900-8565-99DD00A2CBA8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{777D4B16-1D72-40AA-B887-76D98BE3379A}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="14025" xr2:uid="{59BCA3FF-72BC-474B-B1E8-44B9F2CAD3C1}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="14030" xr2:uid="{59BCA3FF-72BC-474B-B1E8-44B9F2CAD3C1}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="28">
   <si>
     <t>Rejestracja</t>
   </si>
@@ -36,9 +36,6 @@
     <t>The E-mail field is not a valid e-mail address</t>
   </si>
   <si>
-    <t>Nie wiem gdzie znaleźć</t>
-  </si>
-  <si>
     <t>The Imię i Nazwisko field is required.</t>
   </si>
   <si>
@@ -106,6 +103,12 @@
   </si>
   <si>
     <t>Błąd przy tworzeniu nowej ankiety</t>
+  </si>
+  <si>
+    <t>Już wiesz</t>
+  </si>
+  <si>
+    <t>Poprawione</t>
   </si>
 </sst>
 </file>
@@ -131,12 +134,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -151,12 +160,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -180,16 +192,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>419100</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>6350</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>527050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1133628</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>53</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1101878</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>342953</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -218,8 +230,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1609725" y="2133600"/>
-          <a:ext cx="1095528" cy="381053"/>
+          <a:off x="6350" y="1263650"/>
+          <a:ext cx="1095528" cy="368353"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -528,26 +540,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEDD963B-E6DF-4B42-A13E-98937FA4006B}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.140625" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="23.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.1796875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.453125" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -555,126 +568,129 @@
         <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="B6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C6" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="B12" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="1" t="s">
+      <c r="C12" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="B13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="1" t="s">
+    </row>
+    <row r="14" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B11" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B12" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B13" s="1" t="s">
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B15" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B15" s="1" t="s">
-        <v>26</v>
+      <c r="D15" s="3" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>